<commit_message>
moved gen python file to data folder, done with data gen
</commit_message>
<xml_diff>
--- a/data/budgeted_user_data.xlsx
+++ b/data/budgeted_user_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pallavitangirala/Documents/projects/budget-recommender/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CB8199-BD75-3848-A081-CAD3ACDD5E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A073C2F3-07B4-8344-A6D5-D8E7BBFC40B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="20000" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4780" yWindow="760" windowWidth="20000" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_data" sheetId="1" r:id="rId1"/>
@@ -1198,9 +1198,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG501"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2040,259 +2040,379 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="7">
         <v>145351</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="7">
         <v>12112</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="7">
         <v>69.5</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="7">
         <v>44.7</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="7">
         <v>67</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>2</v>
-      </c>
-      <c r="N12">
-        <v>2</v>
-      </c>
-      <c r="P12">
-        <v>2</v>
-      </c>
-      <c r="R12">
-        <v>2</v>
-      </c>
-      <c r="T12">
-        <v>3</v>
-      </c>
-      <c r="V12">
-        <v>3</v>
+      <c r="H12" s="7">
+        <v>1</v>
+      </c>
+      <c r="I12" s="7">
+        <v>3028</v>
+      </c>
+      <c r="J12" s="7">
+        <v>1</v>
+      </c>
+      <c r="K12" s="7">
+        <v>1816.8</v>
+      </c>
+      <c r="L12" s="7">
+        <v>2</v>
+      </c>
+      <c r="M12" s="7">
+        <v>1362.6</v>
+      </c>
+      <c r="N12" s="7">
+        <v>2</v>
+      </c>
+      <c r="O12" s="7">
+        <v>163</v>
+      </c>
+      <c r="P12" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>1816.8</v>
+      </c>
+      <c r="R12" s="7">
+        <v>2</v>
+      </c>
+      <c r="S12" s="7">
+        <v>605.6</v>
+      </c>
+      <c r="T12" s="7">
+        <v>3</v>
+      </c>
+      <c r="U12" s="7">
+        <v>2000</v>
+      </c>
+      <c r="V12" s="7">
+        <v>3</v>
+      </c>
+      <c r="W12" s="7">
+        <v>1319.2</v>
       </c>
       <c r="X12" s="7">
         <f t="shared" si="0"/>
-        <v>12112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="7">
         <v>82319</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="7">
         <v>6859</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="7">
         <v>75.3</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="7">
         <v>37.299999999999997</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="7">
         <v>73</v>
       </c>
-      <c r="H13">
-        <v>2</v>
-      </c>
-      <c r="J13">
-        <v>3</v>
-      </c>
-      <c r="L13">
-        <v>2</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-      <c r="R13">
-        <v>3</v>
-      </c>
-      <c r="T13">
-        <v>3</v>
-      </c>
-      <c r="V13">
-        <v>2</v>
+      <c r="H13" s="7">
+        <v>2</v>
+      </c>
+      <c r="I13" s="7">
+        <v>1028.4000000000001</v>
+      </c>
+      <c r="J13" s="7">
+        <v>3</v>
+      </c>
+      <c r="K13" s="7">
+        <v>685.9</v>
+      </c>
+      <c r="L13" s="7">
+        <v>2</v>
+      </c>
+      <c r="M13" s="7">
+        <v>1028.8499999999999</v>
+      </c>
+      <c r="N13" s="7">
+        <v>1</v>
+      </c>
+      <c r="O13" s="7">
+        <v>200</v>
+      </c>
+      <c r="P13" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>1028.8499999999999</v>
+      </c>
+      <c r="R13" s="7">
+        <v>3</v>
+      </c>
+      <c r="S13" s="7">
+        <v>342.95</v>
+      </c>
+      <c r="T13" s="7">
+        <v>3</v>
+      </c>
+      <c r="U13" s="7">
+        <v>1028.8499999999999</v>
+      </c>
+      <c r="V13" s="7">
+        <v>2</v>
+      </c>
+      <c r="W13" s="7">
+        <v>1515.2</v>
       </c>
       <c r="X13" s="7">
         <f t="shared" si="0"/>
-        <v>6859</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="7">
         <v>349974</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="7">
         <v>29164</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="7">
         <v>100</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="7">
         <v>100</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="7">
         <v>100</v>
       </c>
-      <c r="H14">
-        <v>3</v>
-      </c>
-      <c r="J14">
-        <v>3</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="N14">
-        <v>3</v>
-      </c>
-      <c r="P14">
-        <v>2</v>
-      </c>
-      <c r="R14">
-        <v>1</v>
-      </c>
-      <c r="T14">
-        <v>1</v>
-      </c>
-      <c r="V14">
-        <v>2</v>
+      <c r="H14" s="7">
+        <v>3</v>
+      </c>
+      <c r="I14" s="7">
+        <v>4374</v>
+      </c>
+      <c r="J14" s="7">
+        <v>3</v>
+      </c>
+      <c r="K14" s="7">
+        <v>400</v>
+      </c>
+      <c r="L14" s="7">
+        <v>1</v>
+      </c>
+      <c r="M14" s="7">
+        <v>4374.6000000000004</v>
+      </c>
+      <c r="N14" s="7">
+        <v>3</v>
+      </c>
+      <c r="O14" s="7">
+        <v>300</v>
+      </c>
+      <c r="P14" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>4374</v>
+      </c>
+      <c r="R14" s="7">
+        <v>1</v>
+      </c>
+      <c r="S14" s="7">
+        <v>2916.4</v>
+      </c>
+      <c r="T14" s="7">
+        <v>1</v>
+      </c>
+      <c r="U14" s="7">
+        <v>8749.2000000000007</v>
+      </c>
+      <c r="V14" s="7">
+        <v>2</v>
+      </c>
+      <c r="W14" s="7">
+        <v>3675.8</v>
       </c>
       <c r="X14" s="7">
         <f t="shared" si="0"/>
-        <v>29164</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="7">
         <v>1306</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="7">
         <v>108</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="7">
         <v>85</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="7">
         <v>73</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="7">
         <v>81</v>
       </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="N15">
-        <v>2</v>
-      </c>
-      <c r="P15">
-        <v>2</v>
-      </c>
-      <c r="R15">
-        <v>2</v>
-      </c>
-      <c r="T15">
-        <v>2</v>
-      </c>
-      <c r="V15">
-        <v>2</v>
+      <c r="H15" s="7">
+        <v>2</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0</v>
+      </c>
+      <c r="J15" s="7">
+        <v>1</v>
+      </c>
+      <c r="K15" s="7">
+        <v>15</v>
+      </c>
+      <c r="L15" s="7">
+        <v>1</v>
+      </c>
+      <c r="M15" s="7">
+        <v>70</v>
+      </c>
+      <c r="N15" s="7">
+        <v>2</v>
+      </c>
+      <c r="O15" s="7">
+        <v>0</v>
+      </c>
+      <c r="P15" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>0</v>
+      </c>
+      <c r="R15" s="7">
+        <v>2</v>
+      </c>
+      <c r="S15" s="7">
+        <v>0</v>
+      </c>
+      <c r="T15" s="7">
+        <v>2</v>
+      </c>
+      <c r="U15" s="7">
+        <v>23</v>
+      </c>
+      <c r="V15" s="7">
+        <v>2</v>
+      </c>
+      <c r="W15" s="7">
+        <v>0</v>
       </c>
       <c r="X15" s="7">
         <f t="shared" si="0"/>
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>56673</v>
-      </c>
-      <c r="C16">
-        <v>4722</v>
-      </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16">
+      <c r="B16" s="7">
+        <v>19352</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1612</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="7">
+        <v>79.8</v>
+      </c>
+      <c r="F16" s="7">
+        <v>58.3</v>
+      </c>
+      <c r="G16" s="7">
+        <v>77</v>
+      </c>
+      <c r="H16" s="7">
+        <v>2</v>
+      </c>
+      <c r="I16" s="7">
+        <v>564.20000000000005</v>
+      </c>
+      <c r="J16" s="7">
+        <v>3</v>
+      </c>
+      <c r="K16" s="7">
+        <v>200</v>
+      </c>
+      <c r="L16" s="7">
+        <v>1</v>
+      </c>
+      <c r="M16" s="7">
+        <v>216</v>
+      </c>
+      <c r="N16" s="7">
+        <v>2</v>
+      </c>
+      <c r="O16" s="7">
         <v>100</v>
       </c>
-      <c r="F16">
+      <c r="P16" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>161.19999999999999</v>
+      </c>
+      <c r="R16" s="7">
+        <v>2</v>
+      </c>
+      <c r="S16" s="7">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="T16" s="7">
+        <v>3</v>
+      </c>
+      <c r="U16" s="7">
         <v>100</v>
       </c>
-      <c r="G16">
-        <v>100</v>
-      </c>
-      <c r="H16">
-        <v>2</v>
-      </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <v>3</v>
-      </c>
-      <c r="N16">
-        <v>2</v>
-      </c>
-      <c r="P16">
-        <v>2</v>
-      </c>
-      <c r="R16">
-        <v>1</v>
-      </c>
-      <c r="T16">
-        <v>2</v>
-      </c>
-      <c r="V16">
-        <v>1</v>
+      <c r="V16" s="7">
+        <v>2</v>
+      </c>
+      <c r="W16" s="7">
+        <v>190</v>
       </c>
       <c r="X16" s="7">
-        <f t="shared" si="0"/>
-        <v>4722</v>
+        <f>C16-SUM(I16,K16,M16,O16,Q16,S16,U16,W16)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
@@ -2300,50 +2420,50 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>19352</v>
+        <v>56673</v>
       </c>
       <c r="C17">
-        <v>1612</v>
+        <v>4722</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E17">
-        <v>79.8</v>
+        <v>100</v>
       </c>
       <c r="F17">
-        <v>58.3</v>
+        <v>100</v>
       </c>
       <c r="G17">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="H17">
         <v>2</v>
       </c>
       <c r="J17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N17">
         <v>2</v>
       </c>
       <c r="P17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X17" s="7">
         <f t="shared" si="0"/>
-        <v>1612</v>
+        <v>4722</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">

</xml_diff>